<commit_message>
Bài 31 - TestListener
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginData.xlsx
+++ b/src/test/resources/testdata/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\SeleniumJava\Course_SeleniumJava_042023\SeleniumTestNGParallel042023\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80146BC2-0312-4E91-9BFD-EE51A0B53B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA27FDDE-9FFE-43C2-AC99-052B649A2672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{E6AAC135-D369-4C5D-9D40-42DEAC3C870A}"/>
   </bookViews>
@@ -434,7 +434,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>

</xml_diff>